<commit_message>
Final fix of weibull unit case for testing.
</commit_message>
<xml_diff>
--- a/tests/fixtures/weibull/concept.xlsx
+++ b/tests/fixtures/weibull/concept.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\tests\fixtures\weibull\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C70322-C714-460B-9482-F2D1EB5B56ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A89FC18-89C3-4F94-8D94-5157EE7DECD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weibull_dist" sheetId="2" r:id="rId1"/>
@@ -1643,64 +1643,64 @@
                 <c:formatCode>0.00;\-0.00;\-</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>27.215686274509803</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.7058823529411757</c:v>
+                  <c:v>15.941176470588236</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.352941176470587</c:v>
+                  <c:v>17.411764705882355</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.8039215686273273E-2</c:v>
+                  <c:v>17.431372549019606</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-1.2351231148954867E-15</c:v>
+                  <c:v>17.431372549019606</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-1.2351231148954867E-15</c:v>
+                  <c:v>17.431372549019606</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-1.2351231148954867E-15</c:v>
+                  <c:v>17.431372549019606</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-1.2351231148954867E-15</c:v>
+                  <c:v>17.431372549019606</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-1.2351231148954867E-15</c:v>
+                  <c:v>17.431372549019606</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-1.2351231148954867E-15</c:v>
+                  <c:v>17.431372549019606</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-1.2351231148954867E-15</c:v>
+                  <c:v>17.431372549019606</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-1.2351231148954867E-15</c:v>
+                  <c:v>17.431372549019606</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-1.2351231148954867E-15</c:v>
+                  <c:v>17.431372549019606</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-1.2351231148954867E-15</c:v>
+                  <c:v>17.431372549019606</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1745,64 +1745,64 @@
                 <c:formatCode>0.00;\-0.00;\-</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>29.797979797979799</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>31.393939393939394</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>32.18181818181818</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.9</c:v>
+                  <c:v>31.333535353535353</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.8000000000000007</c:v>
+                  <c:v>28.243030303030302</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.5</c:v>
+                  <c:v>24.284444444444446</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8.9</c:v>
+                  <c:v>22.428080808080807</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8</c:v>
+                  <c:v>23.22</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.6</c:v>
+                  <c:v>24.54</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.6999999999999993</c:v>
+                  <c:v>25.479999999999997</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.6999999999999993</c:v>
+                  <c:v>26.02</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.0999999999999992</c:v>
+                  <c:v>26.24</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.29999999999999916</c:v>
+                  <c:v>26.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-8.3266726846886741E-16</c:v>
+                  <c:v>26.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-8.3266726846886741E-16</c:v>
+                  <c:v>26.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-8.3266726846886741E-16</c:v>
+                  <c:v>26.299999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6464,7 +6464,7 @@
   <dimension ref="A1:AY85"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+      <selection activeCell="Q38" sqref="Q38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6574,10 +6574,10 @@
         <v>34</v>
       </c>
       <c r="D10" s="4">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E10" s="4">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:51" x14ac:dyDescent="0.35">
@@ -6701,10 +6701,10 @@
         <v>1</v>
       </c>
       <c r="G15" s="14">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H15" s="14">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="J15" s="6">
         <f t="array" ref="J15:J34">MMULT(AF40:AY59,G15:G34)</f>
@@ -6724,10 +6724,10 @@
       </c>
       <c r="P15" s="6">
         <f t="array" ref="P15:Q34">D10:E10+MMULT(AF15:AY34,(G15:H34-J15:K34-M15:N34))</f>
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="Q15" s="6">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="S15" s="6">
         <f t="array" ref="S15:T34">ROUND((D4:E4/D7:E7)*(C15:C34/D7:E7)^(D4:E4-1)*EXP(-((C15:C34/D7:E7)^D4:E4)),2)</f>
@@ -6824,10 +6824,10 @@
         <v>2</v>
       </c>
       <c r="G16" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H16" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J16" s="6">
         <v>0</v>
@@ -6842,10 +6842,10 @@
         <v>0</v>
       </c>
       <c r="P16" s="6">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="Q16" s="6">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="S16" s="6">
         <v>0</v>
@@ -6937,10 +6937,10 @@
         <v>3</v>
       </c>
       <c r="G17" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H17" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J17" s="6">
         <v>0</v>
@@ -6955,10 +6955,10 @@
         <v>0</v>
       </c>
       <c r="P17" s="6">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="Q17" s="6">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="S17" s="6">
         <v>0</v>
@@ -7050,10 +7050,10 @@
         <v>4</v>
       </c>
       <c r="G18" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H18" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J18" s="6">
         <v>0</v>
@@ -7062,16 +7062,16 @@
         <v>0</v>
       </c>
       <c r="M18" s="6">
-        <v>0</v>
+        <v>0.78431372549019607</v>
       </c>
       <c r="N18" s="6">
         <v>0</v>
       </c>
       <c r="P18" s="6">
-        <v>10</v>
+        <v>27.215686274509803</v>
       </c>
       <c r="Q18" s="6">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="S18" s="6">
         <v>0.06</v>
@@ -7163,10 +7163,10 @@
         <v>5</v>
       </c>
       <c r="G19" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H19" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J19" s="6">
         <v>0</v>
@@ -7175,16 +7175,16 @@
         <v>0</v>
       </c>
       <c r="M19" s="6">
-        <v>0</v>
+        <v>19.215686274509803</v>
       </c>
       <c r="N19" s="6">
-        <v>0</v>
+        <v>0.20202020202020204</v>
       </c>
       <c r="P19" s="6">
         <v>10</v>
       </c>
       <c r="Q19" s="6">
-        <v>10</v>
+        <v>29.797979797979799</v>
       </c>
       <c r="S19" s="6">
         <v>1.47</v>
@@ -7276,10 +7276,10 @@
         <v>6</v>
       </c>
       <c r="G20" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H20" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J20" s="6">
         <v>0</v>
@@ -7291,13 +7291,13 @@
         <v>0</v>
       </c>
       <c r="N20" s="6">
-        <v>0</v>
+        <v>0.40404040404040409</v>
       </c>
       <c r="P20" s="6">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="Q20" s="6">
-        <v>10</v>
+        <v>31.393939393939394</v>
       </c>
       <c r="S20" s="6">
         <v>0</v>
@@ -7389,10 +7389,10 @@
         <v>7</v>
       </c>
       <c r="G21" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H21" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J21" s="6">
         <v>0</v>
@@ -7404,13 +7404,13 @@
         <v>0</v>
       </c>
       <c r="N21" s="6">
-        <v>0</v>
+        <v>1.2121212121212122</v>
       </c>
       <c r="P21" s="6">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="Q21" s="6">
-        <v>10</v>
+        <v>32.18181818181818</v>
       </c>
       <c r="S21" s="6">
         <v>0</v>
@@ -7502,28 +7502,28 @@
         <v>8</v>
       </c>
       <c r="G22" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H22" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J22" s="6">
-        <v>0.29411764705882354</v>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="K22" s="6">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="M22" s="6">
         <v>0</v>
       </c>
       <c r="N22" s="6">
-        <v>0</v>
+        <v>2.8282828282828287</v>
       </c>
       <c r="P22" s="6">
-        <v>9.7058823529411757</v>
+        <v>15.941176470588236</v>
       </c>
       <c r="Q22" s="6">
-        <v>9.9</v>
+        <v>31.333535353535353</v>
       </c>
       <c r="S22" s="6">
         <v>0</v>
@@ -7615,28 +7615,28 @@
         <v>9</v>
       </c>
       <c r="G23" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H23" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J23" s="6">
-        <v>2.3529411764705883</v>
+        <v>0.52941176470588236</v>
       </c>
       <c r="K23" s="6">
-        <v>0.1</v>
+        <v>0.04</v>
       </c>
       <c r="M23" s="6">
         <v>0</v>
       </c>
       <c r="N23" s="6">
-        <v>0</v>
+        <v>5.0505050505050511</v>
       </c>
       <c r="P23" s="6">
-        <v>7.352941176470587</v>
+        <v>17.411764705882355</v>
       </c>
       <c r="Q23" s="6">
-        <v>9.8000000000000007</v>
+        <v>28.243030303030302</v>
       </c>
       <c r="S23" s="6">
         <v>0</v>
@@ -7728,28 +7728,28 @@
         <v>10</v>
       </c>
       <c r="G24" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H24" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J24" s="6">
-        <v>7.2549019607843137</v>
+        <v>1.9803921568627449</v>
       </c>
       <c r="K24" s="6">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="M24" s="6">
         <v>0</v>
       </c>
       <c r="N24" s="6">
-        <v>0</v>
+        <v>5.8585858585858581</v>
       </c>
       <c r="P24" s="6">
-        <v>9.8039215686273273E-2</v>
+        <v>17.431372549019606</v>
       </c>
       <c r="Q24" s="6">
-        <v>9.5</v>
+        <v>24.284444444444446</v>
       </c>
       <c r="S24" s="6">
         <v>0</v>
@@ -7841,28 +7841,28 @@
         <v>11</v>
       </c>
       <c r="G25" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H25" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J25" s="6">
-        <v>9.8039215686274508E-2</v>
+        <v>1.9999999999999998</v>
       </c>
       <c r="K25" s="6">
-        <v>0.6</v>
+        <v>0.21999999999999997</v>
       </c>
       <c r="M25" s="6">
         <v>0</v>
       </c>
       <c r="N25" s="6">
-        <v>0</v>
+        <v>3.6363636363636367</v>
       </c>
       <c r="P25" s="6">
-        <v>-1.2351231148954867E-15</v>
+        <v>17.431372549019606</v>
       </c>
       <c r="Q25" s="6">
-        <v>8.9</v>
+        <v>22.428080808080807</v>
       </c>
       <c r="S25" s="6">
         <v>0</v>
@@ -7954,28 +7954,28 @@
         <v>12</v>
       </c>
       <c r="G26" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H26" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J26" s="6">
-        <v>0</v>
+        <v>1.9999999999999998</v>
       </c>
       <c r="K26" s="6">
-        <v>0.89999999999999991</v>
+        <v>0.4</v>
       </c>
       <c r="M26" s="6">
         <v>0</v>
       </c>
       <c r="N26" s="6">
-        <v>0</v>
+        <v>0.80808080808080818</v>
       </c>
       <c r="P26" s="6">
-        <v>-1.2351231148954867E-15</v>
+        <v>17.431372549019606</v>
       </c>
       <c r="Q26" s="6">
-        <v>8</v>
+        <v>23.22</v>
       </c>
       <c r="S26" s="6">
         <v>0</v>
@@ -8067,16 +8067,16 @@
         <v>13</v>
       </c>
       <c r="G27" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H27" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J27" s="6">
-        <v>0</v>
+        <v>1.9999999999999998</v>
       </c>
       <c r="K27" s="6">
-        <v>1.4000000000000001</v>
+        <v>0.68000000000000016</v>
       </c>
       <c r="M27" s="6">
         <v>0</v>
@@ -8085,10 +8085,10 @@
         <v>0</v>
       </c>
       <c r="P27" s="6">
-        <v>-1.2351231148954867E-15</v>
+        <v>17.431372549019606</v>
       </c>
       <c r="Q27" s="6">
-        <v>6.6</v>
+        <v>24.54</v>
       </c>
       <c r="S27" s="6">
         <v>0</v>
@@ -8180,16 +8180,16 @@
         <v>14</v>
       </c>
       <c r="G28" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H28" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J28" s="6">
-        <v>0</v>
+        <v>1.9999999999999998</v>
       </c>
       <c r="K28" s="6">
-        <v>1.9</v>
+        <v>1.06</v>
       </c>
       <c r="M28" s="6">
         <v>0</v>
@@ -8198,10 +8198,10 @@
         <v>0</v>
       </c>
       <c r="P28" s="6">
-        <v>-1.2351231148954867E-15</v>
+        <v>17.431372549019606</v>
       </c>
       <c r="Q28" s="6">
-        <v>4.6999999999999993</v>
+        <v>25.479999999999997</v>
       </c>
       <c r="S28" s="6">
         <v>0</v>
@@ -8293,16 +8293,16 @@
         <v>15</v>
       </c>
       <c r="G29" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H29" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J29" s="6">
-        <v>0</v>
+        <v>1.9999999999999998</v>
       </c>
       <c r="K29" s="6">
-        <v>2</v>
+        <v>1.46</v>
       </c>
       <c r="M29" s="6">
         <v>0</v>
@@ -8311,10 +8311,10 @@
         <v>0</v>
       </c>
       <c r="P29" s="6">
-        <v>-1.2351231148954867E-15</v>
+        <v>17.431372549019606</v>
       </c>
       <c r="Q29" s="6">
-        <v>2.6999999999999993</v>
+        <v>26.02</v>
       </c>
       <c r="S29" s="6">
         <v>0</v>
@@ -8406,16 +8406,16 @@
         <v>16</v>
       </c>
       <c r="G30" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H30" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J30" s="6">
-        <v>0</v>
+        <v>1.9999999999999998</v>
       </c>
       <c r="K30" s="6">
-        <v>1.6</v>
+        <v>1.7800000000000002</v>
       </c>
       <c r="M30" s="6">
         <v>0</v>
@@ -8424,10 +8424,10 @@
         <v>0</v>
       </c>
       <c r="P30" s="6">
-        <v>-1.2351231148954867E-15</v>
+        <v>17.431372549019606</v>
       </c>
       <c r="Q30" s="6">
-        <v>1.0999999999999992</v>
+        <v>26.24</v>
       </c>
       <c r="S30" s="6">
         <v>0</v>
@@ -8519,16 +8519,16 @@
         <v>17</v>
       </c>
       <c r="G31" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H31" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J31" s="6">
-        <v>0</v>
+        <v>1.9999999999999998</v>
       </c>
       <c r="K31" s="6">
-        <v>0.8</v>
+        <v>1.94</v>
       </c>
       <c r="M31" s="6">
         <v>0</v>
@@ -8537,10 +8537,10 @@
         <v>0</v>
       </c>
       <c r="P31" s="6">
-        <v>-1.2351231148954867E-15</v>
+        <v>17.431372549019606</v>
       </c>
       <c r="Q31" s="6">
-        <v>0.29999999999999916</v>
+        <v>26.299999999999997</v>
       </c>
       <c r="S31" s="6">
         <v>0</v>
@@ -8632,16 +8632,16 @@
         <v>18</v>
       </c>
       <c r="G32" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H32" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J32" s="6">
-        <v>0</v>
+        <v>1.9999999999999998</v>
       </c>
       <c r="K32" s="6">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="M32" s="6">
         <v>0</v>
@@ -8650,10 +8650,10 @@
         <v>0</v>
       </c>
       <c r="P32" s="6">
-        <v>-1.2351231148954867E-15</v>
+        <v>17.431372549019606</v>
       </c>
       <c r="Q32" s="6">
-        <v>-8.3266726846886741E-16</v>
+        <v>26.299999999999997</v>
       </c>
       <c r="S32" s="6">
         <v>0</v>
@@ -8745,16 +8745,16 @@
         <v>19</v>
       </c>
       <c r="G33" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H33" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J33" s="6">
-        <v>0</v>
+        <v>1.9999999999999998</v>
       </c>
       <c r="K33" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M33" s="6">
         <v>0</v>
@@ -8763,10 +8763,10 @@
         <v>0</v>
       </c>
       <c r="P33" s="6">
-        <v>-1.2351231148954867E-15</v>
+        <v>17.431372549019606</v>
       </c>
       <c r="Q33" s="6">
-        <v>-8.3266726846886741E-16</v>
+        <v>26.299999999999997</v>
       </c>
       <c r="S33" s="6">
         <v>0</v>
@@ -8858,16 +8858,16 @@
         <v>20</v>
       </c>
       <c r="G34" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H34" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J34" s="6">
-        <v>0</v>
+        <v>1.9999999999999998</v>
       </c>
       <c r="K34" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M34" s="6">
         <v>0</v>
@@ -8876,10 +8876,10 @@
         <v>0</v>
       </c>
       <c r="P34" s="6">
-        <v>-1.2351231148954867E-15</v>
+        <v>17.431372549019606</v>
       </c>
       <c r="Q34" s="6">
-        <v>-8.3266726846886741E-16</v>
+        <v>26.299999999999997</v>
       </c>
       <c r="S34" s="6">
         <v>0</v>
@@ -8969,27 +8969,27 @@
     <row r="36" spans="3:51" x14ac:dyDescent="0.35">
       <c r="G36" s="7">
         <f>SUM(G15:G34)</f>
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="H36" s="7">
         <f>SUM(H15:H34)</f>
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="J36" s="7">
         <f>SUM(J15:J34)</f>
-        <v>10</v>
+        <v>22.56862745098039</v>
       </c>
       <c r="K36" s="7">
         <f>SUM(K15:K34)</f>
-        <v>10.000000000000002</v>
+        <v>13.700000000000001</v>
       </c>
       <c r="M36" s="7">
         <f>SUM(M15:M34)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="N36" s="7">
         <f>SUM(N15:N34)</f>
-        <v>0</v>
+        <v>20.000000000000004</v>
       </c>
       <c r="P36" s="15"/>
       <c r="Q36" s="15"/>

</xml_diff>